<commit_message>
Q2 plan & Design
</commit_message>
<xml_diff>
--- a/Q1/time_log.xlsx
+++ b/Q1/time_log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdw12_000\Desktop\Ara\BCPR280_SoftwareEngineering2\Assignment1_Due03052019\Q1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdw12_000\Desktop\Ara\BCPR280_Part1\Q1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA8BF6C-97DA-467C-B1C3-F1D3091D71D8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4219E70-3A60-479A-9AFC-4022D3341067}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9885" yWindow="2430" windowWidth="18330" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10470" yWindow="945" windowWidth="18330" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>PSP Time Recording Log</t>
   </si>
@@ -377,6 +377,34 @@
   </si>
   <si>
     <t>Drawing a design level class diagram &amp; Activity diagram</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coding</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Starting code based on design</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Continue on coding</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Starting test for code</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found some issues and the way to fix</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Testing</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixing code and try to separate classes, Controller &amp; Model</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -995,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1102,6 +1130,108 @@
       </c>
       <c r="H8" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="14">
+        <v>43549</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="F9" s="15">
+        <v>0.96388888888888891</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="14">
+        <v>43553</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0.9819444444444444</v>
+      </c>
+      <c r="F10" s="15">
+        <v>0.50902777777777775</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="14">
+        <v>43554</v>
+      </c>
+      <c r="D11" s="15">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="F11" s="15">
+        <v>4.7916666666666663E-2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="14">
+        <v>43554</v>
+      </c>
+      <c r="D12" s="15">
+        <v>0.62430555555555556</v>
+      </c>
+      <c r="F12" s="15">
+        <v>0.64166666666666672</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="14">
+        <v>43554</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0.66875000000000007</v>
+      </c>
+      <c r="F13" s="15">
+        <v>0.68888888888888899</v>
+      </c>
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="14">
+        <v>43556</v>
+      </c>
+      <c r="D14" s="15">
+        <v>0.70347222222222217</v>
+      </c>
+      <c r="F14" s="15">
+        <v>0.74583333333333324</v>
+      </c>
+      <c r="H14" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>